<commit_message>
add group bar charts2
</commit_message>
<xml_diff>
--- a/writings/fig/Hbayes_experiment_result.xlsx
+++ b/writings/fig/Hbayes_experiment_result.xlsx
@@ -8,13 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhexuanxu/Documents/GitHub/hierarchical_bayesian/writings/fig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2208F7DF-6A67-C34F-BA89-E934CFF2F5C3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{978B34DA-567A-D048-86C1-236099FFEFA3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41440" yWindow="5420" windowWidth="28100" windowHeight="17440" xr2:uid="{7D0F4819-6D81-CA46-98EF-D8B1237CC229}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">工作表1!$G$37</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">工作表1!$G$38</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">工作表1!$H$38:$K$38</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">工作表1!$H$39:$K$39</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">工作表1!$H$40:$K$40</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">工作表1!$H$41:$K$41</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">工作表1!$H$42:$K$42</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">工作表1!$H$43:$K$43</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">工作表1!$H$44:$K$44</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">工作表1!$G$39</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">工作表1!$G$40</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">工作表1!$G$41</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">工作表1!$G$42</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">工作表1!$G$43</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">工作表1!$G$44</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">工作表1!$H$36:$K$36</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">工作表1!$H$37:$K$37</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -848,7 +867,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1300" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -897,7 +916,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -907,18 +926,26 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100" b="1"/>
+                  <a:rPr lang="en-US" sz="1400" b="1">
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
                   <a:t>F1</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="zh-Hans" sz="1100" b="1"/>
+                  <a:rPr lang="zh-Hans" sz="1400" b="1">
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
                   <a:t> </a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100" b="1"/>
+                  <a:rPr lang="en-US" sz="1400" b="1">
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
                   <a:t>Score</a:t>
                 </a:r>
-                <a:endParaRPr lang="zh-CN" sz="1100" b="1"/>
+                <a:endParaRPr lang="zh-CN" sz="1400" b="1">
+                  <a:latin typeface="+mn-lt"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -935,7 +962,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -1688,7 +1715,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -1736,7 +1763,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -1746,7 +1773,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1200" b="1">
+                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1400" b="1">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -1754,7 +1781,7 @@
                   </a:rPr>
                   <a:t>Precision</a:t>
                 </a:r>
-                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -1776,7 +1803,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -1805,7 +1832,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2531,7 +2558,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -2578,7 +2605,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -2588,7 +2615,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -2596,14 +2623,14 @@
                   <a:t>R</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1200" b="1">
+                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1400" b="1">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>ecall</a:t>
                 </a:r>
-                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -2624,7 +2651,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -2653,7 +2680,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3385,7 +3412,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1300" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -3433,7 +3460,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -3446,7 +3473,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1">
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -3454,7 +3481,7 @@
                   <a:t>F</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1100" b="1">
+                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1400" b="1">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -3462,7 +3489,7 @@
                   <a:t>1</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="zh-Hans" altLang="en-US" sz="1100" b="1" baseline="0">
+                  <a:rPr lang="zh-Hans" altLang="en-US" sz="1400" b="1" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -3470,14 +3497,14 @@
                   <a:t> </a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1100" b="1" baseline="0">
+                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1400" b="1" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>Score</a:t>
                 </a:r>
-                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1">
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -3498,7 +3525,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -3530,7 +3557,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4263,7 +4290,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -4312,7 +4339,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -4325,7 +4352,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -4333,14 +4360,14 @@
                   <a:t>P</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1200" b="1">
+                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1400" b="1">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>recision</a:t>
                 </a:r>
-                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -4361,7 +4388,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -4393,7 +4420,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5126,7 +5153,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -5173,7 +5200,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -5186,7 +5213,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1">
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -5194,14 +5221,14 @@
                   <a:t>R</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1200" b="1">
+                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1400" b="1">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
                   <a:t>ecall</a:t>
                 </a:r>
-                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1">
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
@@ -5222,7 +5249,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -5254,7 +5281,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -5272,6 +5299,869 @@
         <c:crossAx val="1099455439"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$G$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CoClustering</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$H$25:$K$25</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>pre@5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>pre@10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>pre@25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>pre@50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$H$26:$K$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.0499999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6299999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9500000000000002E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D6EC-5142-B307-136530505999}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$G$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NMF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$H$25:$K$25</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>pre@5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>pre@10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>pre@25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>pre@50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$H$27:$K$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.5999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2800000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.1699999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0999999999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D6EC-5142-B307-136530505999}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$G$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVD++ </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$H$25:$K$25</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>pre@5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>pre@10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>pre@25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>pre@50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$H$28:$K$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.3499999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2499999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1299999999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D6EC-5142-B307-136530505999}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$G$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HSR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$H$25:$K$25</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>pre@5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>pre@10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>pre@25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>pre@50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$H$29:$K$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.5499999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2800000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1400000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D6EC-5142-B307-136530505999}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$G$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HPF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$H$25:$K$25</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>pre@5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>pre@10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>pre@25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>pre@50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$H$30:$K$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.6999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3099999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2700000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.21E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D6EC-5142-B307-136530505999}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$G$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$H$25:$K$25</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>pre@5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>pre@10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>pre@25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>pre@50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$H$31:$K$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.6700000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2300000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1700000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D6EC-5142-B307-136530505999}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$G$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LambdaMART</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$H$25:$K$25</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>pre@5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>pre@10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>pre@25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>pre@50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$H$32:$K$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.4300000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3100000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2699999999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-D6EC-5142-B307-136530505999}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$G$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HBayes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>工作表1!$H$25:$K$25</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>pre@5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>pre@10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>pre@25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>pre@50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$H$33:$K$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.6799999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3400000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-D6EC-5142-B307-136530505999}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1136661759"/>
+        <c:axId val="1136669759"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1136661759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1136669759"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1136669759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="8.0000000000000016E-2"/>
+          <c:min val="4.0000000000000008E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>P</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1400" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>recision</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1136661759"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0000000000000002E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -5591,6 +6481,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -8107,6 +9037,509 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8827,6 +10260,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="图表 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEA993A6-9850-8944-A7CA-86A50655E319}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9129,8 +10598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0B6C1F-DD20-7C49-BF06-48E60A9A7B26}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H12" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+    <sheetView tabSelected="1" topLeftCell="H33" workbookViewId="0">
+      <selection activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>